<commit_message>
App, scrum en alles
</commit_message>
<xml_diff>
--- a/Documenten/Backlogs Project 4.xlsx
+++ b/Documenten/Backlogs Project 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rogier\Documenten\INFPRJ 4-2\INFPRJ-004\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8156E-B32A-42C4-9B3A-B4D1D9399730}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828BE53B-5B75-4842-AE24-04BE20539E59}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t>Category</t>
   </si>
@@ -194,6 +194,38 @@
     <t>1. Schrijf code die 3 random foute antwoorden genereert bij de gegenereerde sommetjes en 1 correct antwoord.
 2. Bij correct antwoord: naar de volgende som en 1 punt toekennen
 3. Bij fout antwoord: 1 'leven' minder (wanneer 3 levens verbruikt zijn, beëindig de opdracht)</t>
+  </si>
+  <si>
+    <t>Score / reeks</t>
+  </si>
+  <si>
+    <t>Levens / kansen</t>
+  </si>
+  <si>
+    <t>Als een user wil ik zien hoeveel ik goed heb of mijn score zien, zodat ik mijn voortgang kan bekijken en mij te motiveren om door te gaan.</t>
+  </si>
+  <si>
+    <t>1. Schrijf code voor levens.
+2. Wanneer de gebruiker 0 levens over heeft, beëindig de sommen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wanneer de gebruiker 0 levens over heeft, beëindig de sommen. Laat de levens zien op het oefenscherm.</t>
+  </si>
+  <si>
+    <t>1. Schijf code voor score.
+2. Laat de score zien op het oefenscherm</t>
+  </si>
+  <si>
+    <t>Als een user wil ik zien hoeveel levens / kansen ik nog heb.</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Inlog</t>
+  </si>
+  <si>
+    <t>Verschillende oefenmodussen</t>
   </si>
 </sst>
 </file>
@@ -648,7 +680,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,22 +908,52 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
+      <c r="B18" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
+      <c r="B19" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -983,7 +1045,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,20 +1165,42 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="13"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="12"/>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>

</xml_diff>

<commit_message>
Scrum + console app delete
Scrum is klaar, project is bijna klaar!!
</commit_message>
<xml_diff>
--- a/Documenten/Backlogs Project 4.xlsx
+++ b/Documenten/Backlogs Project 4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rogier\Documenten\INFPRJ 4-2\INFPRJ-004\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828BE53B-5B75-4842-AE24-04BE20539E59}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4644CC3E-8314-4713-B03F-795C5D0374D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Category</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Rekensommetjes controleren</t>
   </si>
   <si>
-    <t>Verschillende rekenopdrachten (+ / - / % )</t>
-  </si>
-  <si>
     <t>Uitleg- / Over ons-pagina</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Geluidjes / achtergrondmuziek</t>
   </si>
   <si>
-    <t>Instellingen: kleurenblindmodus, geluid aan/uit</t>
-  </si>
-  <si>
     <t>Als een user wil ik met rekensommetjes oefenen.</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
   </si>
   <si>
     <t>Als een user wil ik weten wie de app developers zijn.</t>
-  </si>
-  <si>
-    <t>1. Schrijf een Over/About pagina</t>
   </si>
   <si>
     <t>1. Schrijf code die wallpapers unlockt wanneer de gebruiker 10 keer een goed antwoord geeft.
@@ -222,10 +213,85 @@
     <t>Ranking</t>
   </si>
   <si>
-    <t>Inlog</t>
-  </si>
-  <si>
-    <t>Verschillende oefenmodussen</t>
+    <t>Verschillende rekenopdrachten (+ / - )</t>
+  </si>
+  <si>
+    <t>Als een user wil ik een kleurenblindmodus hebben zodat wanneer ik minder moeite heb met de kleuren te onderscheiden als ik kleurenblind ben.</t>
+  </si>
+  <si>
+    <t>0,5 u</t>
+  </si>
+  <si>
+    <t>0,2 u</t>
+  </si>
+  <si>
+    <t>1. Schrijf een Over/About pagina
+2. Maak een knop op het hoofdmenu die navigeert naar de About pagina</t>
+  </si>
+  <si>
+    <t>Er is een werkende knop die naar de About pagina leidt. Op de About pagina zijn de gegevens te vinden van de developers en PO.</t>
+  </si>
+  <si>
+    <t>1. Implementeer code waardoor je de thema van de app kan veranderen.
+2. Implementeer dat je deze modus via een knop in de instellingen kan veranderen in het hoofdmenu.</t>
+  </si>
+  <si>
+    <t>Wanneer de kleurenblindmodus aan is, zijn alle kleuren zo veranderd, dat mensen die moeite hebben met kleur zien alsnog de kleuren uit elkaar kunnen halen. De thema moet heel de app aanpassen.</t>
+  </si>
+  <si>
+    <t>Instellingen: kleurenblindmodus</t>
+  </si>
+  <si>
+    <t>Als een user wil ik een app die een mooie lay-out heeft, zodat ik meer gestimuleerd en aangetrokken ben om de app te gebruiken.</t>
+  </si>
+  <si>
+    <t>1. Voeg een titel en afbeelding toe op het hoofdmenu.</t>
+  </si>
+  <si>
+    <t>Er is een afbeelding in het hoofdmenu.</t>
+  </si>
+  <si>
+    <t>Als een user wil ik geluid en achtergrondmuziek, zodat ik de app leuker en aangenamer vindt tijdens het gebruiken.</t>
+  </si>
+  <si>
+    <t>1 u</t>
+  </si>
+  <si>
+    <t>1. Vind bijpassende achtergrondmuziek en sound FX's. 
+2. Implementeer dit in het oefenscherm.
+3. Implementeer dat je geluiden hoort wanneer een goed en fout antwoord wordt gegeven.</t>
+  </si>
+  <si>
+    <t>De geluiden zijn hoorbaar bij het geven van antwoorden in het oefenscherm. Ook is er achtergrondmuziek te horen tijdens het oefenen.</t>
+  </si>
+  <si>
+    <t>Als een user wil ik een highscore, zodat ik gemotiveerder ben om meer goede antwoorden te geven tijdens het oefenen.</t>
+  </si>
+  <si>
+    <t>1. Implementeer code waardoor de highscore ziet per oefenmodus.
+2. Implementeer de code in het scherm waar gebruikers de oefenmodi selecteren.</t>
+  </si>
+  <si>
+    <t>De highscore is zichtbaar in het scherm waar gebruikers de oefenmodi selecteren. De highscore slaat op en laat dezelfde gegevens zien als de app weer opgestart wordt. De highscore update wanneer er een betere score is behaald.</t>
+  </si>
+  <si>
+    <t>Als een user wil ik kunnen inloggen met een account, zodat ik mijn gegevens en scores kan personaliseren.</t>
+  </si>
+  <si>
+    <t>1. Stel een database in.
+2. Implementeer code die de database linkt met de app.
+3. Implementeer code die gebruikers een account kan aanmaken.
+4. Implementeer code die gebruikers laat inloggen.
+5. Implementeer code die de scores van de gebruikers opslaat op de accounts.</t>
+  </si>
+  <si>
+    <t>Gebruikers kunnen makkelijk een account aanmaken. Ook is het mogelijk om in te loggen. Wanneer zij inloggen kunnen zij makkelijk zien  wat hun behaalde scores zijn. Uitloggen is ook mogelijk.</t>
+  </si>
+  <si>
+    <t>Inloggen via database</t>
+  </si>
+  <si>
+    <t>2 u</t>
   </si>
 </sst>
 </file>
@@ -679,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
@@ -754,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>6</v>
@@ -770,10 +836,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -786,7 +852,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>6</v>
@@ -802,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
@@ -816,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>15</v>
@@ -832,7 +898,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>6</v>
@@ -848,7 +914,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>6</v>
@@ -864,10 +930,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -880,7 +946,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>6</v>
@@ -896,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>18</v>
@@ -912,7 +978,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>6</v>
@@ -927,33 +993,46 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
       <c r="B18" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="B19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,7 +1044,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,16 +1085,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
       <c r="E3" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1023,16 +1105,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
       <c r="E4" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1130,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,10 +1172,10 @@
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>6</v>
@@ -1099,10 +1184,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1110,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>6</v>
@@ -1119,10 +1204,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1130,7 +1215,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>6</v>
@@ -1139,10 +1224,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1150,7 +1235,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>6</v>
@@ -1159,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1170,7 +1255,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>6</v>
@@ -1179,7 +1264,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1187,19 +1272,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" s="9">
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,55 +1373,125 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="12"/>
+      <c r="A5" s="14">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>

</xml_diff>